<commit_message>
analysis.py and more gis resources
</commit_message>
<xml_diff>
--- a/data/riv_data.xlsx
+++ b/data/riv_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Travail\Modèle Sescousse\modele_sescousse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA1813-F2F2-442A-8731-64857A4073DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254F2AF0-F1EE-4C01-A660-EB9D5AD9FDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23256" yWindow="2304" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11566,7 +11566,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11739,8 +11739,8 @@
         <v>0.08</v>
       </c>
       <c r="E9">
-        <f>E6+0.01*C6*D6</f>
-        <v>20.195899999999998</v>
+        <f>E6</f>
+        <v>20.1312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>